<commit_message>
[mrunal] Add. Added pakages and releases to Flipkart Application
</commit_message>
<xml_diff>
--- a/FlipkartData.xlsx
+++ b/FlipkartData.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA_Projects\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0088D8-7323-489C-A5CE-1D2757A47F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -55,13 +49,16 @@
   </si>
   <si>
     <t>Apple iPhone 11 Pro (Midnight Green, 256 GB)</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,26 +361,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:E9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="45.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +390,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -405,7 +405,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -416,7 +416,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -427,7 +427,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -438,7 +438,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>